<commit_message>
Suicides graph in italy
</commit_message>
<xml_diff>
--- a/data/suicidi.xlsx
+++ b/data/suicidi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maidi\OneDrive\Desktop\rProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F5353-3A0D-449D-9283-9D2E8EACB6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CFEC6E-C121-4941-9C49-90FC379C3D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1820,22 +1820,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1844,13 +1835,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -3410,7 +3410,7 @@
   <dimension ref="A2:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H25"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="9.6" x14ac:dyDescent="0.2"/>
@@ -3428,16 +3428,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="131" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
     </row>
     <row r="3" spans="1:8" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="130" t="s">
@@ -4190,14 +4190,14 @@
       <c r="P2" s="42"/>
     </row>
     <row r="3" spans="1:21" s="8" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="137"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
+      <c r="B3" s="134"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
@@ -4207,69 +4207,69 @@
     </row>
     <row r="4" spans="1:21" s="38" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="39"/>
-      <c r="B4" s="138"/>
-      <c r="C4" s="138"/>
+      <c r="B4" s="135"/>
+      <c r="C4" s="135"/>
     </row>
     <row r="5" spans="1:21" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="133" t="s">
+      <c r="A5" s="136" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="139" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="140"/>
-      <c r="D5" s="140"/>
-      <c r="E5" s="140"/>
-      <c r="F5" s="140"/>
-      <c r="G5" s="140"/>
-      <c r="H5" s="140"/>
-      <c r="I5" s="140"/>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
-      <c r="L5" s="140"/>
-      <c r="M5" s="140"/>
-      <c r="N5" s="140"/>
-      <c r="O5" s="140"/>
-      <c r="P5" s="140"/>
-      <c r="Q5" s="140"/>
-      <c r="R5" s="140"/>
-      <c r="S5" s="140"/>
-      <c r="T5" s="140"/>
-      <c r="U5" s="141" t="s">
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="139"/>
+      <c r="J5" s="139"/>
+      <c r="K5" s="139"/>
+      <c r="L5" s="139"/>
+      <c r="M5" s="139"/>
+      <c r="N5" s="139"/>
+      <c r="O5" s="139"/>
+      <c r="P5" s="139"/>
+      <c r="Q5" s="139"/>
+      <c r="R5" s="139"/>
+      <c r="S5" s="139"/>
+      <c r="T5" s="139"/>
+      <c r="U5" s="140" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="139"/>
-      <c r="B6" s="135" t="s">
+      <c r="A6" s="137"/>
+      <c r="B6" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="141"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="141"/>
+      <c r="G6" s="141"/>
       <c r="H6" s="34"/>
-      <c r="I6" s="135" t="s">
+      <c r="I6" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
+      <c r="J6" s="141"/>
+      <c r="K6" s="141"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="141"/>
+      <c r="N6" s="141"/>
       <c r="O6" s="34"/>
-      <c r="P6" s="136" t="s">
+      <c r="P6" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="Q6" s="136"/>
-      <c r="R6" s="136"/>
-      <c r="S6" s="136"/>
-      <c r="T6" s="136"/>
-      <c r="U6" s="131"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="132"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="132"/>
+      <c r="U6" s="133"/>
     </row>
     <row r="7" spans="1:21" s="61" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="134"/>
+      <c r="A7" s="138"/>
       <c r="B7" s="52" t="s">
         <v>66</v>
       </c>
@@ -4323,7 +4323,7 @@
       <c r="T7" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="U7" s="135"/>
+      <c r="U7" s="141"/>
     </row>
     <row r="8" spans="1:21" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
@@ -4371,28 +4371,28 @@
       <c r="U9" s="34"/>
     </row>
     <row r="10" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="131" t="s">
+      <c r="B10" s="133" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="131"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
-      <c r="H10" s="131"/>
-      <c r="I10" s="131"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="131"/>
-      <c r="L10" s="131"/>
-      <c r="M10" s="131"/>
-      <c r="N10" s="131"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
-      <c r="Q10" s="131"/>
-      <c r="R10" s="131"/>
-      <c r="S10" s="131"/>
-      <c r="T10" s="131"/>
-      <c r="U10" s="131"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="133"/>
+      <c r="M10" s="133"/>
+      <c r="N10" s="133"/>
+      <c r="O10" s="133"/>
+      <c r="P10" s="133"/>
+      <c r="Q10" s="133"/>
+      <c r="R10" s="133"/>
+      <c r="S10" s="133"/>
+      <c r="T10" s="133"/>
+      <c r="U10" s="133"/>
     </row>
     <row r="11" spans="1:21" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="43" t="s">
@@ -8511,14 +8511,14 @@
       <c r="AG2" s="42"/>
     </row>
     <row r="3" spans="1:33" s="8" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="134" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="137"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
+      <c r="B3" s="134"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
@@ -8527,14 +8527,14 @@
       <c r="L3" s="41"/>
       <c r="M3" s="41"/>
       <c r="N3" s="41"/>
-      <c r="R3" s="137" t="s">
+      <c r="R3" s="134" t="s">
         <v>61</v>
       </c>
-      <c r="S3" s="137"/>
-      <c r="T3" s="137"/>
-      <c r="U3" s="137"/>
-      <c r="V3" s="137"/>
-      <c r="W3" s="137"/>
+      <c r="S3" s="134"/>
+      <c r="T3" s="134"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="134"/>
       <c r="X3" s="41"/>
       <c r="Y3" s="41"/>
       <c r="Z3" s="41"/>
@@ -8546,11 +8546,11 @@
     </row>
     <row r="4" spans="1:33" s="38" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40"/>
-      <c r="B4" s="138"/>
-      <c r="C4" s="138"/>
+      <c r="B4" s="135"/>
+      <c r="C4" s="135"/>
       <c r="R4" s="39"/>
-      <c r="S4" s="138"/>
-      <c r="T4" s="138"/>
+      <c r="S4" s="135"/>
+      <c r="T4" s="135"/>
     </row>
     <row r="5" spans="1:33" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
@@ -12332,6 +12332,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="S24:AG24"/>
+    <mergeCell ref="S37:AG37"/>
+    <mergeCell ref="S38:AG38"/>
+    <mergeCell ref="R3:W3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S7:AG7"/>
+    <mergeCell ref="S9:AG9"/>
+    <mergeCell ref="S23:AG23"/>
     <mergeCell ref="B37:P37"/>
     <mergeCell ref="B7:P7"/>
     <mergeCell ref="B38:P38"/>
@@ -12340,14 +12348,6 @@
     <mergeCell ref="B24:P24"/>
     <mergeCell ref="B9:P9"/>
     <mergeCell ref="B23:P23"/>
-    <mergeCell ref="S24:AG24"/>
-    <mergeCell ref="S37:AG37"/>
-    <mergeCell ref="S38:AG38"/>
-    <mergeCell ref="R3:W3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="S7:AG7"/>
-    <mergeCell ref="S9:AG9"/>
-    <mergeCell ref="S23:AG23"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>

</xml_diff>